<commit_message>
Fiz alguns use cases
</commit_message>
<xml_diff>
--- a/UseCase/Descrição UseCases/ComprarCarro.xlsx
+++ b/UseCase/Descrição UseCases/ComprarCarro.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\UseCase\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\UseCase\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0B2D02-1520-4118-BA58-C0A63EF503C3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="25440" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="25440" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Actor input</t>
   </si>
@@ -55,12 +54,15 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Estar registado no sistema</t>
-  </si>
-  <si>
     <t>Carro encomendado</t>
   </si>
   <si>
+    <t>Estar autenticado no sistema</t>
+  </si>
+  <si>
+    <t>Alternativa 2 [Escolher Especificações] (passo 6)</t>
+  </si>
+  <si>
     <t>1. &lt;&lt;include&gt;&gt; Fazer Login</t>
   </si>
   <si>
@@ -70,43 +72,43 @@
     <t>3. Indica que quer comprar carro</t>
   </si>
   <si>
+    <t>5. Seleciona modelo que pretende comprar</t>
+  </si>
+  <si>
     <t>4. Mostra todos os modelos disponiveis</t>
   </si>
   <si>
-    <t>5. Seleciona modelo que pretende comprar</t>
-  </si>
-  <si>
-    <t>6. Pergunta qual a forma de personalizar o carro</t>
-  </si>
-  <si>
-    <t>7. Escolhe configuração ótima</t>
-  </si>
-  <si>
-    <t>8.&lt;&lt;include&gt;&gt; Escolher configuração otima</t>
-  </si>
-  <si>
-    <t>Alternativa 1 [Escolher Pacote] (passo 7)</t>
-  </si>
-  <si>
-    <t>7.1 Escolhe Pacote</t>
-  </si>
-  <si>
-    <t>7.2 &lt;&lt;include&gt;&gt; Escolhe Pacote</t>
-  </si>
-  <si>
-    <t>Alternativa 2 [Escolher Especificações] (passo 7)</t>
-  </si>
-  <si>
-    <t>7.1 Escolhe Especificações</t>
-  </si>
-  <si>
-    <t>7.2 &lt;&lt;include&gt;&gt; Escolher Especificações</t>
+    <t>6. Regista opção</t>
+  </si>
+  <si>
+    <t>7. Pergunta qual a forma de personalizar o carro</t>
+  </si>
+  <si>
+    <t>8. Escolhe configuração ótima</t>
+  </si>
+  <si>
+    <t>9.&lt;&lt;include&gt;&gt; Escolher configuração ótima</t>
+  </si>
+  <si>
+    <t>Alternativa 1 [Escolher Pacote] (passo 8)</t>
+  </si>
+  <si>
+    <t>8.1 Escolhe Pacote</t>
+  </si>
+  <si>
+    <t>8.2 &lt;&lt;include&gt;&gt; Escolhe Pacote</t>
+  </si>
+  <si>
+    <t>8.1 Escolhe Especificações</t>
+  </si>
+  <si>
+    <t>8.2 &lt;&lt;include&gt;&gt; Escolher Especificações</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -336,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -354,6 +356,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -375,8 +380,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,11 +699,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -705,45 +714,45 @@
     <col min="5" max="5" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="C5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -753,123 +762,131 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="19"/>
-      <c r="C8" s="5"/>
+    <row r="7" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="21"/>
+      <c r="C7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="22"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="22"/>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="19"/>
+    <row r="10" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="22"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="19"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="22"/>
       <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
+    <row r="12" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="22"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="19"/>
-      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="19"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="13" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="22"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="19"/>
+    <row r="14" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="22"/>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="22"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="19"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="22"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="13"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1" t="s">
+      <c r="B18" s="16" t="s">
         <v>21</v>
       </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="13"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="10"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="21" t="s">
+      <c r="B21" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="16"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B6:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>